<commit_message>
Moved all transformation into transform_attributes
</commit_message>
<xml_diff>
--- a/out/factor_values_2.xlsx
+++ b/out/factor_values_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Factor</t>
+          <t>factor</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>value</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Dissatisfied_ratio</t>
+          <t>dissatisfied_ratio</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Satisfied_count</t>
+          <t>satisfied_count</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Dissatisfied_count</t>
+          <t>dissatisfied_count</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>probability</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>chi</t>
         </is>
       </c>
     </row>
@@ -472,19 +482,25 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05340519353258207</v>
+        <v>0.7808641975308642</v>
       </c>
       <c r="D2" t="n">
-        <v>11592</v>
+        <v>213</v>
       </c>
       <c r="E2" t="n">
-        <v>654</v>
+        <v>759</v>
       </c>
       <c r="F2" t="n">
-        <v>12246</v>
+        <v>972</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4986.45091038875</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +510,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7813141683778234</v>
+        <v>0.05341706083836242</v>
       </c>
       <c r="D3" t="n">
-        <v>213</v>
+        <v>11607</v>
       </c>
       <c r="E3" t="n">
-        <v>761</v>
+        <v>655</v>
       </c>
       <c r="F3" t="n">
-        <v>974</v>
+        <v>12262</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6.544473228086024e-98</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4986.45091038875</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +538,25 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03933364183248496</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D4" t="n">
-        <v>2076</v>
+        <v>152</v>
       </c>
       <c r="E4" t="n">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="F4" t="n">
-        <v>2161</v>
+        <v>288</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1077.099187338824</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +566,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04887337353221199</v>
+        <v>0.3072060682680152</v>
       </c>
       <c r="D5" t="n">
-        <v>2997</v>
+        <v>548</v>
       </c>
       <c r="E5" t="n">
-        <v>154</v>
+        <v>243</v>
       </c>
       <c r="F5" t="n">
-        <v>3151</v>
+        <v>791</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1077.099187338824</v>
       </c>
     </row>
     <row r="6">
@@ -560,19 +594,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>0.07872928176795579</v>
+        <v>0.1593030491599253</v>
       </c>
       <c r="D6" t="n">
-        <v>3335</v>
+        <v>2702</v>
       </c>
       <c r="E6" t="n">
-        <v>285</v>
+        <v>512</v>
       </c>
       <c r="F6" t="n">
-        <v>3620</v>
+        <v>3214</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1077.099187338824</v>
       </c>
     </row>
     <row r="7">
@@ -582,19 +622,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1599127182044888</v>
+        <v>0.07836644591611479</v>
       </c>
       <c r="D7" t="n">
-        <v>2695</v>
+        <v>3340</v>
       </c>
       <c r="E7" t="n">
-        <v>513</v>
+        <v>284</v>
       </c>
       <c r="F7" t="n">
-        <v>3208</v>
+        <v>3624</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4.21433618393792e-09</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1077.099187338824</v>
       </c>
     </row>
     <row r="8">
@@ -604,19 +650,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3059418457648546</v>
+        <v>0.04884237234379955</v>
       </c>
       <c r="D8" t="n">
-        <v>549</v>
+        <v>2999</v>
       </c>
       <c r="E8" t="n">
-        <v>242</v>
+        <v>154</v>
       </c>
       <c r="F8" t="n">
-        <v>791</v>
+        <v>3153</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.453946301150233e-31</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1077.099187338824</v>
       </c>
     </row>
     <row r="9">
@@ -626,67 +678,81 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.03927911275415896</v>
       </c>
       <c r="D9" t="n">
-        <v>153</v>
+        <v>2079</v>
       </c>
       <c r="E9" t="n">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="F9" t="n">
-        <v>289</v>
+        <v>2164</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.346911670100846e-31</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1077.099187338824</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sla_result</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Achieved</t>
-        </is>
+          <t>sla_breached</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.07605192089903302</v>
+        <v>0.3117106773823192</v>
       </c>
       <c r="D10" t="n">
-        <v>10606</v>
+        <v>1199</v>
       </c>
       <c r="E10" t="n">
-        <v>873</v>
+        <v>543</v>
       </c>
       <c r="F10" t="n">
-        <v>11479</v>
+        <v>1742</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>879.782667854151</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>sla_result</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Breached</t>
-        </is>
+          <t>sla_breached</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3113153360137852</v>
+        <v>0.0757918552036199</v>
       </c>
       <c r="D11" t="n">
-        <v>1199</v>
+        <v>10621</v>
       </c>
       <c r="E11" t="n">
-        <v>542</v>
+        <v>871</v>
       </c>
       <c r="F11" t="n">
-        <v>1741</v>
+        <v>11492</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7.812338348741308e-30</v>
+      </c>
+      <c r="H11" t="n">
+        <v>879.782667854151</v>
       </c>
     </row>
     <row r="12">
@@ -696,19 +762,25 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C12" t="n">
-        <v>0.08597807270628967</v>
+        <v>0.3744075829383886</v>
       </c>
       <c r="D12" t="n">
-        <v>6336</v>
+        <v>132</v>
       </c>
       <c r="E12" t="n">
-        <v>596</v>
+        <v>79</v>
       </c>
       <c r="F12" t="n">
-        <v>6932</v>
+        <v>211</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>340.4283166328635</v>
       </c>
     </row>
     <row r="13">
@@ -718,19 +790,25 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1044045676998369</v>
+        <v>0.265017667844523</v>
       </c>
       <c r="D13" t="n">
-        <v>4392</v>
+        <v>208</v>
       </c>
       <c r="E13" t="n">
-        <v>512</v>
+        <v>75</v>
       </c>
       <c r="F13" t="n">
-        <v>4904</v>
+        <v>283</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.9999999999999731</v>
+      </c>
+      <c r="H13" t="n">
+        <v>340.4283166328635</v>
       </c>
     </row>
     <row r="14">
@@ -743,16 +821,22 @@
         <v>2</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1707865168539326</v>
+        <v>0.17152466367713</v>
       </c>
       <c r="D14" t="n">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="E14" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F14" t="n">
-        <v>890</v>
+        <v>892</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9999999977984574</v>
+      </c>
+      <c r="H14" t="n">
+        <v>340.4283166328635</v>
       </c>
     </row>
     <row r="15">
@@ -762,19 +846,25 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2685512367491166</v>
+        <v>0.1042982277449582</v>
       </c>
       <c r="D15" t="n">
-        <v>207</v>
+        <v>4397</v>
       </c>
       <c r="E15" t="n">
-        <v>76</v>
+        <v>512</v>
       </c>
       <c r="F15" t="n">
-        <v>283</v>
+        <v>4909</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.2909728463082871</v>
+      </c>
+      <c r="H15" t="n">
+        <v>340.4283166328635</v>
       </c>
     </row>
     <row r="16">
@@ -784,19 +874,25 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3744075829383886</v>
+        <v>0.08574722582504683</v>
       </c>
       <c r="D16" t="n">
-        <v>132</v>
+        <v>6344</v>
       </c>
       <c r="E16" t="n">
-        <v>79</v>
+        <v>595</v>
       </c>
       <c r="F16" t="n">
-        <v>211</v>
+        <v>6939</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2.546909737157177e-09</v>
+      </c>
+      <c r="H16" t="n">
+        <v>340.4283166328635</v>
       </c>
     </row>
     <row r="17">
@@ -807,20 +903,26 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Data Correction</t>
+          <t>No Resolution Action</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.04909240924092409</v>
+        <v>0.1696741179639106</v>
       </c>
       <c r="D17" t="n">
-        <v>2305</v>
+        <v>3083</v>
       </c>
       <c r="E17" t="n">
-        <v>119</v>
+        <v>630</v>
       </c>
       <c r="F17" t="n">
-        <v>2424</v>
+        <v>3713</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="18">
@@ -831,20 +933,26 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Environmental Restoration</t>
+          <t>Information Provided / Training</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.05952380952380952</v>
+        <v>0.1089574708317651</v>
       </c>
       <c r="D18" t="n">
-        <v>158</v>
+        <v>4735</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>579</v>
       </c>
       <c r="F18" t="n">
-        <v>168</v>
+        <v>5314</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.7001015665287339</v>
+      </c>
+      <c r="H18" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="19">
@@ -855,20 +963,26 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Information Provided / Training</t>
+          <t>Environmental Restoration</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.109622641509434</v>
+        <v>0.05952380952380952</v>
       </c>
       <c r="D19" t="n">
-        <v>4719</v>
+        <v>158</v>
       </c>
       <c r="E19" t="n">
-        <v>581</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
-        <v>5300</v>
+        <v>168</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.02475911987982579</v>
+      </c>
+      <c r="H19" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="20">
@@ -879,20 +993,26 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>No Resolution Action</t>
+          <t>Security Modification</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.1692266235516033</v>
+        <v>0.05570291777188329</v>
       </c>
       <c r="D20" t="n">
-        <v>3083</v>
+        <v>712</v>
       </c>
       <c r="E20" t="n">
-        <v>628</v>
+        <v>42</v>
       </c>
       <c r="F20" t="n">
-        <v>3711</v>
+        <v>754</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5.613066757188756e-07</v>
+      </c>
+      <c r="H20" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="21">
@@ -903,20 +1023,26 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Reboot / Restart</t>
+          <t>Software Correction</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.02863436123348018</v>
+        <v>0.05339805825242718</v>
       </c>
       <c r="D21" t="n">
-        <v>441</v>
+        <v>390</v>
       </c>
       <c r="E21" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F21" t="n">
-        <v>454</v>
+        <v>412</v>
+      </c>
+      <c r="G21" t="n">
+        <v>9.660615690617236e-05</v>
+      </c>
+      <c r="H21" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="22">
@@ -927,20 +1053,26 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Security Modification</t>
+          <t>Data Correction</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.05577689243027888</v>
+        <v>0.0487603305785124</v>
       </c>
       <c r="D22" t="n">
-        <v>711</v>
+        <v>2302</v>
       </c>
       <c r="E22" t="n">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="F22" t="n">
-        <v>753</v>
+        <v>2420</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1.063722824419134e-24</v>
+      </c>
+      <c r="H22" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="23">
@@ -951,140 +1083,166 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Software Correction</t>
+          <t>Reboot / Restart</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.05365853658536585</v>
+        <v>0.02869757174392936</v>
       </c>
       <c r="D23" t="n">
-        <v>388</v>
+        <v>440</v>
       </c>
       <c r="E23" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F23" t="n">
-        <v>410</v>
+        <v>453</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3.634237019319601e-10</v>
+      </c>
+      <c r="H23" t="n">
+        <v>315.57622820523</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>sla_priority</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Priority 2</t>
-        </is>
+          <t>priority_is_4</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>0.03125</v>
+        <v>0.1293998480628007</v>
       </c>
       <c r="D24" t="n">
-        <v>31</v>
+        <v>6876</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>1022</v>
       </c>
       <c r="F24" t="n">
-        <v>32</v>
+        <v>7898</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9999999998740063</v>
+      </c>
+      <c r="H24" t="n">
+        <v>103.8263314178949</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>sla_priority</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Priority 3</t>
-        </is>
+          <t>priority_is_4</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>0.07375966798717223</v>
+        <v>0.0734632683658171</v>
       </c>
       <c r="D25" t="n">
-        <v>4910</v>
+        <v>4944</v>
       </c>
       <c r="E25" t="n">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F25" t="n">
-        <v>5301</v>
+        <v>5336</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5.927722361686574e-17</v>
+      </c>
+      <c r="H25" t="n">
+        <v>103.8263314178949</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>sla_priority</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Priority 4</t>
-        </is>
+          <t>caller_is_employee</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1297071129707113</v>
+        <v>0.1245384357166835</v>
       </c>
       <c r="D26" t="n">
-        <v>6864</v>
+        <v>7824</v>
       </c>
       <c r="E26" t="n">
-        <v>1023</v>
+        <v>1113</v>
       </c>
       <c r="F26" t="n">
-        <v>7887</v>
+        <v>8937</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.9999999458238565</v>
+      </c>
+      <c r="H26" t="n">
+        <v>89.71333796111035</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>caller_employee_type</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>employees</t>
-        </is>
+          <t>caller_is_employee</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1245101332437577</v>
+        <v>0.07004887130556202</v>
       </c>
       <c r="D27" t="n">
-        <v>7819</v>
+        <v>3996</v>
       </c>
       <c r="E27" t="n">
-        <v>1112</v>
+        <v>301</v>
       </c>
       <c r="F27" t="n">
-        <v>8931</v>
+        <v>4297</v>
+      </c>
+      <c r="G27" t="n">
+        <v>8.505400932930321e-17</v>
+      </c>
+      <c r="H27" t="n">
+        <v>89.71333796111035</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>caller_employee_type</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>partners</t>
-        </is>
+          <t>incident_has_ka_related_flag</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
       </c>
       <c r="C28" t="n">
-        <v>0.07049486461251167</v>
+        <v>0.1231512666569044</v>
       </c>
       <c r="D28" t="n">
-        <v>3982</v>
+        <v>5988</v>
       </c>
       <c r="E28" t="n">
-        <v>302</v>
+        <v>841</v>
       </c>
       <c r="F28" t="n">
-        <v>4284</v>
+        <v>6829</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.9999912202740207</v>
+      </c>
+      <c r="H28" t="n">
+        <v>38.95749777616205</v>
       </c>
     </row>
     <row r="29">
@@ -1094,41 +1252,53 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1228919196363103</v>
+        <v>0.08946135831381732</v>
       </c>
       <c r="D29" t="n">
-        <v>5981</v>
+        <v>5832</v>
       </c>
       <c r="E29" t="n">
-        <v>838</v>
+        <v>573</v>
       </c>
       <c r="F29" t="n">
-        <v>6819</v>
+        <v>6405</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2.185298888607617e-06</v>
+      </c>
+      <c r="H29" t="n">
+        <v>38.95749777616205</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>incident_has_ka_related_flag</t>
+          <t>self_service</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>0.09014216528667396</v>
+        <v>0.1476846057571965</v>
       </c>
       <c r="D30" t="n">
-        <v>5824</v>
+        <v>1362</v>
       </c>
       <c r="E30" t="n">
-        <v>577</v>
+        <v>236</v>
       </c>
       <c r="F30" t="n">
-        <v>6401</v>
+        <v>1598</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.999999807077853</v>
+      </c>
+      <c r="H30" t="n">
+        <v>31.27813668428506</v>
       </c>
     </row>
     <row r="31">
@@ -1138,41 +1308,25 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>0.147777082028804</v>
+        <v>0.1012375386730835</v>
       </c>
       <c r="D31" t="n">
-        <v>1361</v>
+        <v>10458</v>
       </c>
       <c r="E31" t="n">
-        <v>236</v>
+        <v>1178</v>
       </c>
       <c r="F31" t="n">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>self_service</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.1014368063322722</v>
-      </c>
-      <c r="D32" t="n">
-        <v>10444</v>
-      </c>
-      <c r="E32" t="n">
-        <v>1179</v>
-      </c>
-      <c r="F32" t="n">
-        <v>11623</v>
+        <v>11636</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.02531359593991387</v>
+      </c>
+      <c r="H31" t="n">
+        <v>31.27813668428506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>